<commit_message>
Sheet menu selesai ditambahkan
</commit_message>
<xml_diff>
--- a/Template Data v4.xlsx
+++ b/Template Data v4.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="746">
   <si>
     <t>Nama</t>
   </si>
@@ -1876,6 +1876,396 @@
   </si>
   <si>
     <t>tambahan makanan</t>
+  </si>
+  <si>
+    <t>express special 1 (nasi goreng rainbow)</t>
+  </si>
+  <si>
+    <t>express special 2 (kwetiau goreng rainbow)</t>
+  </si>
+  <si>
+    <t>express special 3 (mie goreng rainbow)</t>
+  </si>
+  <si>
+    <t>express special 4 (capcay + nasi sweet hot/ice rainbow tea</t>
+  </si>
+  <si>
+    <t>express special 5 (nasi + chicken crispy + capcay + clear soup bakso polos (2pcs) sweet hot/ice rainbow tea</t>
+  </si>
+  <si>
+    <t>bakpao ayam</t>
+  </si>
+  <si>
+    <t>kaki ayam</t>
+  </si>
+  <si>
+    <t>hakau</t>
+  </si>
+  <si>
+    <t>siomay special</t>
+  </si>
+  <si>
+    <t>enoki crispy</t>
+  </si>
+  <si>
+    <t>kulit ayam crispy</t>
+  </si>
+  <si>
+    <t>chicken karaage</t>
+  </si>
+  <si>
+    <t>deep fried gyoza</t>
+  </si>
+  <si>
+    <t>pan fried gyoza</t>
+  </si>
+  <si>
+    <t>chicken katsu</t>
+  </si>
+  <si>
+    <t>chicken teriyaki</t>
+  </si>
+  <si>
+    <t>beef teriyaki</t>
+  </si>
+  <si>
+    <t>fish katsu</t>
+  </si>
+  <si>
+    <t>tempura moriawase</t>
+  </si>
+  <si>
+    <t>gohan</t>
+  </si>
+  <si>
+    <t>chicken chasiu</t>
+  </si>
+  <si>
+    <t>chicken katsu don</t>
+  </si>
+  <si>
+    <t>fish katsu don</t>
+  </si>
+  <si>
+    <t>sunny don</t>
+  </si>
+  <si>
+    <t>spicy chicken don</t>
+  </si>
+  <si>
+    <t>chasiu don</t>
+  </si>
+  <si>
+    <t>chicken kaarage don</t>
+  </si>
+  <si>
+    <t>chicken teriyaki don</t>
+  </si>
+  <si>
+    <t>beef teriyaki don</t>
+  </si>
+  <si>
+    <t>chicken kaarage set</t>
+  </si>
+  <si>
+    <t>chicken katsu set</t>
+  </si>
+  <si>
+    <t>chicken teriyaki set</t>
+  </si>
+  <si>
+    <t>beef teriyaki set</t>
+  </si>
+  <si>
+    <t>fish katsu set</t>
+  </si>
+  <si>
+    <t>calamari set</t>
+  </si>
+  <si>
+    <t>tempura moriawase set</t>
+  </si>
+  <si>
+    <t>hot plate beef teriyaki</t>
+  </si>
+  <si>
+    <t>hotplate seafood</t>
+  </si>
+  <si>
+    <t>hot plate chicken teriyaki</t>
+  </si>
+  <si>
+    <t>hot plate spicy chicken</t>
+  </si>
+  <si>
+    <t>ebi tempura ramen</t>
+  </si>
+  <si>
+    <t>basic ramen</t>
+  </si>
+  <si>
+    <t>vegetable ramen</t>
+  </si>
+  <si>
+    <t>kani ramen</t>
+  </si>
+  <si>
+    <t>chicken teriyaki ramen</t>
+  </si>
+  <si>
+    <t>beef patty ramen</t>
+  </si>
+  <si>
+    <t>chicken patty ramen</t>
+  </si>
+  <si>
+    <t>tenderloin teriyaki ramen</t>
+  </si>
+  <si>
+    <t>chicken chasiu ramen</t>
+  </si>
+  <si>
+    <t>gyoza ramen</t>
+  </si>
+  <si>
+    <t>sunny ramen</t>
+  </si>
+  <si>
+    <t>agadashi tofu ramen</t>
+  </si>
+  <si>
+    <t>spicy chicken ramen</t>
+  </si>
+  <si>
+    <t>chicken katsu ramen</t>
+  </si>
+  <si>
+    <t>chicken karaage ramen</t>
+  </si>
+  <si>
+    <t>beef patty</t>
+  </si>
+  <si>
+    <t>chicken patty</t>
+  </si>
+  <si>
+    <t>spicy katsu maki</t>
+  </si>
+  <si>
+    <t>california maki</t>
+  </si>
+  <si>
+    <t>tenderloin maki</t>
+  </si>
+  <si>
+    <t>tori kushi no maki</t>
+  </si>
+  <si>
+    <t>kyuri maki</t>
+  </si>
+  <si>
+    <t>tori kani maki</t>
+  </si>
+  <si>
+    <t>kani maki</t>
+  </si>
+  <si>
+    <t>set A (tropical maki, chicken dynamite, spicy katsu maki)</t>
+  </si>
+  <si>
+    <t>set B (california maki, tenderloin maki, tori kushi no maki)</t>
+  </si>
+  <si>
+    <t>tropical maki</t>
+  </si>
+  <si>
+    <t>avocado maki</t>
+  </si>
+  <si>
+    <t>chicken dynamite maki</t>
+  </si>
+  <si>
+    <t>beef dynamite maki</t>
+  </si>
+  <si>
+    <t>yellow taxi</t>
+  </si>
+  <si>
+    <t>red cross</t>
+  </si>
+  <si>
+    <t>marcheepan</t>
+  </si>
+  <si>
+    <t>tropical forest</t>
+  </si>
+  <si>
+    <t>passion fusion</t>
+  </si>
+  <si>
+    <t>cold ocha</t>
+  </si>
+  <si>
+    <t>coca-cola</t>
+  </si>
+  <si>
+    <t>fanta</t>
+  </si>
+  <si>
+    <t>ice chocolate</t>
+  </si>
+  <si>
+    <t>lime squash</t>
+  </si>
+  <si>
+    <t>hot ocha</t>
+  </si>
+  <si>
+    <t>paket A (Beef Patty Donburi + Ramen Salad + Ocha)</t>
+  </si>
+  <si>
+    <t>paket b (kroket donburi + yasaiitame + salad + clear soup + ocha)</t>
+  </si>
+  <si>
+    <t>paket c (chicken patty donburi + agedashi tofu + tekanako maki +  salad  + ocha )</t>
+  </si>
+  <si>
+    <t>paket d (chicken katsu donburi + yasaiitame +  salad + clear soup + Ocha)</t>
+  </si>
+  <si>
+    <t>rotigal</t>
+  </si>
+  <si>
+    <t>tehkotak</t>
+  </si>
+  <si>
+    <t>nu milk tea</t>
+  </si>
+  <si>
+    <t>nu green tea</t>
+  </si>
+  <si>
+    <t>nescafe</t>
+  </si>
+  <si>
+    <t>beef bowl original (regular)</t>
+  </si>
+  <si>
+    <t>beef bowl original (large)</t>
+  </si>
+  <si>
+    <t>beef bowl yakiniku (regular)</t>
+  </si>
+  <si>
+    <t>beef bowl yakiniku (large)</t>
+  </si>
+  <si>
+    <t>beef bowl original egg mayo (regular)</t>
+  </si>
+  <si>
+    <t>beef bowl original egg mayo (large)</t>
+  </si>
+  <si>
+    <t>beef bowl orginal red hot chili (regular)</t>
+  </si>
+  <si>
+    <t>beef bowl original red hot chili (large)</t>
+  </si>
+  <si>
+    <t>beef bowl yakiniku red hot chili (regular)</t>
+  </si>
+  <si>
+    <t>beef bowl yakiniku red hot chili (large)</t>
+  </si>
+  <si>
+    <t>beef bowl original creamy (regular)</t>
+  </si>
+  <si>
+    <t>beef bowl original creamy (large)</t>
+  </si>
+  <si>
+    <t>beef bowl original crispy spinach (regular)</t>
+  </si>
+  <si>
+    <t>beef bowl yakiniku crispy spinach (large)</t>
+  </si>
+  <si>
+    <t>extra topping for beef bowl</t>
+  </si>
+  <si>
+    <t>egg mayo</t>
+  </si>
+  <si>
+    <t>red hot chili</t>
+  </si>
+  <si>
+    <t>creamy</t>
+  </si>
+  <si>
+    <t>crispy spinach</t>
+  </si>
+  <si>
+    <t>veggie beef bowl (reguler)</t>
+  </si>
+  <si>
+    <t>veggie beef bowl (large)</t>
+  </si>
+  <si>
+    <t>teriyaki chicken bowl</t>
+  </si>
+  <si>
+    <t>shrimp bowl</t>
+  </si>
+  <si>
+    <t>ebi fry</t>
+  </si>
+  <si>
+    <t>kaarage</t>
+  </si>
+  <si>
+    <t>crispy ebi</t>
+  </si>
+  <si>
+    <t>shumai</t>
+  </si>
+  <si>
+    <t>katsu</t>
+  </si>
+  <si>
+    <t>shrimp cutlet</t>
+  </si>
+  <si>
+    <t>egg roll</t>
+  </si>
+  <si>
+    <t>beef only (original/yakiniku)</t>
+  </si>
+  <si>
+    <t>teriyaki chicken only</t>
+  </si>
+  <si>
+    <t>vegetable only</t>
+  </si>
+  <si>
+    <t>miso soup</t>
+  </si>
+  <si>
+    <t>paket puas! A (original beef + 2 pcs katsu, 2 pcs shumai atau 1 pcs ebi fry, 1 pcs egg roll, 1 pcs shumai )</t>
+  </si>
+  <si>
+    <t>paket puas! B (yakiniku beef + 2 pcs katsu, 2 pcs shumai atau 1 pcs ebi fry, 1 pcs egg roll, 1 pcs shumai)</t>
+  </si>
+  <si>
+    <t>paket puas! C (veggie beef + 2 pcs katsu, 2 pcs shumai atau 1 pcs ebi fry, 1 pcs egg roll, 1 pcs shumai)</t>
+  </si>
+  <si>
+    <t>paket puas! D (teriyaki chicken + 2 pcs katsu, 2 pcs shumai atau 1 pcs ebi fry, 1 pcs egg roll, 1 pcs shumai)</t>
+  </si>
+  <si>
+    <t>crispy set (4 pcs karage + nasi)</t>
+  </si>
+  <si>
+    <t>Combo (original / yakiniku beef bowl + teriyaki chicken)</t>
   </si>
 </sst>
 </file>
@@ -2010,7 +2400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2091,6 +2481,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3109,8 +3506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O723"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A537" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A553" sqref="A553"/>
+    <sheetView tabSelected="1" topLeftCell="A644" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G663" sqref="G663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3185,7 +3582,7 @@
         <v>27273</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -3207,7 +3604,7 @@
         <v>31818</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3229,7 +3626,7 @@
         <v>29091</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -3251,7 +3648,7 @@
         <v>31818</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -3273,7 +3670,7 @@
         <v>33363</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -3295,7 +3692,7 @@
         <v>30000</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -3317,7 +3714,7 @@
         <v>33363</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -3336,7 +3733,7 @@
         <v>35455</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -3358,7 +3755,7 @@
         <v>27272</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -3380,7 +3777,7 @@
         <v>27273</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -3402,7 +3799,7 @@
         <v>27273</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -3424,7 +3821,7 @@
         <v>27273</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -3446,7 +3843,7 @@
         <v>31818</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -3470,7 +3867,7 @@
         <v>22500</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -3492,7 +3889,7 @@
         <v>17500</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -3515,7 +3912,7 @@
         <v>30000</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -3535,7 +3932,7 @@
         <v>24500</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -3554,7 +3951,7 @@
         <v>19500</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -3573,7 +3970,7 @@
         <v>30000</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -3592,7 +3989,7 @@
         <v>25000</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -3611,7 +4008,7 @@
         <v>20000</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -3630,7 +4027,7 @@
         <v>24500</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
@@ -3649,7 +4046,7 @@
         <v>19500</v>
       </c>
       <c r="D24" s="3"/>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -3668,7 +4065,7 @@
         <v>27000</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -3687,7 +4084,7 @@
         <v>22000</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -3706,7 +4103,7 @@
         <v>22500</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -3725,7 +4122,7 @@
         <v>27500</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -3744,7 +4141,7 @@
         <v>30000</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>1</v>
       </c>
       <c r="F29" s="2" t="s">
@@ -3763,7 +4160,7 @@
         <v>27000</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
@@ -3782,7 +4179,7 @@
         <v>22000</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -3801,7 +4198,7 @@
         <v>24500</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
@@ -3820,7 +4217,7 @@
         <v>19500</v>
       </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
@@ -3839,7 +4236,7 @@
         <v>30000</v>
       </c>
       <c r="D34" s="3"/>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
@@ -3858,7 +4255,7 @@
         <v>24500</v>
       </c>
       <c r="D35" s="3"/>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
@@ -3877,7 +4274,7 @@
         <v>19500</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>1</v>
       </c>
       <c r="F36" s="2" t="s">
@@ -3896,7 +4293,7 @@
         <v>27500</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
@@ -3915,7 +4312,7 @@
         <v>22500</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
@@ -3934,7 +4331,7 @@
         <v>27500</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
@@ -3953,7 +4350,7 @@
         <v>22500</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
@@ -3972,7 +4369,7 @@
         <v>25000</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>1</v>
       </c>
       <c r="F41" s="2" t="s">
@@ -3991,7 +4388,7 @@
         <v>20000</v>
       </c>
       <c r="D42" s="3"/>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
@@ -4010,7 +4407,7 @@
         <v>30000</v>
       </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>1</v>
       </c>
       <c r="F43" s="2" t="s">
@@ -4029,7 +4426,7 @@
         <v>25000</v>
       </c>
       <c r="D44" s="3"/>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>1</v>
       </c>
       <c r="F44" s="2" t="s">
@@ -4048,7 +4445,7 @@
         <v>20000</v>
       </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
@@ -4067,7 +4464,7 @@
         <v>30000</v>
       </c>
       <c r="D46" s="3"/>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>1</v>
       </c>
       <c r="F46" s="2" t="s">
@@ -4086,7 +4483,7 @@
         <v>20000</v>
       </c>
       <c r="D47" s="3"/>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>1</v>
       </c>
       <c r="F47" s="2" t="s">
@@ -4105,7 +4502,7 @@
         <v>25000</v>
       </c>
       <c r="D48" s="3"/>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
@@ -4124,7 +4521,7 @@
         <v>30000</v>
       </c>
       <c r="D49" s="3"/>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>1</v>
       </c>
       <c r="F49" s="2" t="s">
@@ -4143,7 +4540,7 @@
         <v>20000</v>
       </c>
       <c r="D50" s="3"/>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
@@ -4162,7 +4559,7 @@
         <v>25000</v>
       </c>
       <c r="D51" s="3"/>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
@@ -4181,7 +4578,7 @@
         <v>30000</v>
       </c>
       <c r="D52" s="3"/>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
@@ -4200,7 +4597,7 @@
         <v>20000</v>
       </c>
       <c r="D53" s="3"/>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>1</v>
       </c>
       <c r="F53" s="2" t="s">
@@ -13676,1182 +14073,2830 @@
       </c>
     </row>
     <row r="553" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A553" s="17"/>
-      <c r="B553"/>
-      <c r="C553" s="11"/>
+      <c r="A553" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B553" t="s">
+        <v>616</v>
+      </c>
+      <c r="C553">
+        <v>22000</v>
+      </c>
       <c r="D553"/>
-      <c r="E553"/>
-      <c r="G553"/>
+      <c r="E553">
+        <v>1</v>
+      </c>
+      <c r="F553" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G553" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A554" s="17"/>
-      <c r="B554"/>
-      <c r="C554" s="11"/>
+      <c r="B554" t="s">
+        <v>617</v>
+      </c>
+      <c r="C554">
+        <v>22000</v>
+      </c>
       <c r="D554"/>
-      <c r="E554"/>
-      <c r="G554"/>
+      <c r="E554">
+        <v>1</v>
+      </c>
+      <c r="F554" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G554" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A555" s="17"/>
-      <c r="B555"/>
-      <c r="C555" s="11"/>
+      <c r="B555" t="s">
+        <v>618</v>
+      </c>
+      <c r="C555">
+        <v>22000</v>
+      </c>
       <c r="D555"/>
-      <c r="E555"/>
-      <c r="G555"/>
+      <c r="E555">
+        <v>1</v>
+      </c>
+      <c r="F555" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G555" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A556" s="17"/>
-      <c r="B556"/>
-      <c r="C556" s="11"/>
+      <c r="B556" t="s">
+        <v>619</v>
+      </c>
+      <c r="C556">
+        <v>25000</v>
+      </c>
       <c r="D556"/>
-      <c r="E556"/>
-      <c r="G556"/>
+      <c r="E556">
+        <v>1</v>
+      </c>
+      <c r="F556" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G556" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A557" s="17"/>
-      <c r="B557"/>
-      <c r="C557" s="11"/>
+      <c r="B557" t="s">
+        <v>620</v>
+      </c>
+      <c r="C557">
+        <v>25000</v>
+      </c>
       <c r="D557"/>
-      <c r="E557"/>
-      <c r="G557"/>
+      <c r="E557">
+        <v>1</v>
+      </c>
+      <c r="F557" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G557" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="558" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A558" s="17"/>
-      <c r="B558"/>
-      <c r="C558" s="11"/>
+      <c r="B558" t="s">
+        <v>621</v>
+      </c>
+      <c r="C558">
+        <v>12000</v>
+      </c>
       <c r="D558"/>
-      <c r="E558"/>
-      <c r="G558"/>
+      <c r="E558">
+        <v>1</v>
+      </c>
+      <c r="F558" t="s">
+        <v>60</v>
+      </c>
+      <c r="G558" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="559" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A559" s="17"/>
-      <c r="B559"/>
-      <c r="C559" s="11"/>
+      <c r="B559" t="s">
+        <v>622</v>
+      </c>
+      <c r="C559">
+        <v>12000</v>
+      </c>
       <c r="D559"/>
-      <c r="E559"/>
-      <c r="G559"/>
+      <c r="E559">
+        <v>1</v>
+      </c>
+      <c r="F559" t="s">
+        <v>60</v>
+      </c>
+      <c r="G559" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="560" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A560" s="17"/>
-      <c r="B560"/>
-      <c r="C560" s="11"/>
+      <c r="B560" t="s">
+        <v>623</v>
+      </c>
+      <c r="C560">
+        <v>12000</v>
+      </c>
       <c r="D560"/>
-      <c r="E560"/>
-    </row>
-    <row r="561" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E560">
+        <v>1</v>
+      </c>
+      <c r="F560" t="s">
+        <v>60</v>
+      </c>
+      <c r="G560" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="561" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A561" s="17"/>
-      <c r="B561"/>
-      <c r="C561" s="11"/>
+      <c r="B561" t="s">
+        <v>624</v>
+      </c>
+      <c r="C561">
+        <v>12000</v>
+      </c>
       <c r="D561"/>
-      <c r="E561"/>
-    </row>
-    <row r="562" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E561">
+        <v>1</v>
+      </c>
+      <c r="F561" t="s">
+        <v>60</v>
+      </c>
+      <c r="G561" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A562" s="17"/>
-      <c r="B562"/>
-      <c r="C562" s="11"/>
+      <c r="B562" t="s">
+        <v>625</v>
+      </c>
+      <c r="C562">
+        <v>15000</v>
+      </c>
       <c r="D562"/>
-      <c r="E562"/>
-    </row>
-    <row r="563" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E562">
+        <v>1</v>
+      </c>
+      <c r="F562" t="s">
+        <v>60</v>
+      </c>
+      <c r="G562" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="563" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A563" s="17"/>
-      <c r="B563"/>
-      <c r="C563" s="11"/>
+      <c r="B563" t="s">
+        <v>626</v>
+      </c>
+      <c r="C563">
+        <v>12000</v>
+      </c>
       <c r="D563"/>
-      <c r="E563"/>
-    </row>
-    <row r="564" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A564" s="17"/>
-      <c r="B564"/>
-      <c r="C564" s="11"/>
+      <c r="E563">
+        <v>1</v>
+      </c>
+      <c r="F563" t="s">
+        <v>60</v>
+      </c>
+      <c r="G563" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A564" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B564" t="s">
+        <v>627</v>
+      </c>
+      <c r="C564">
+        <v>27800</v>
+      </c>
       <c r="D564"/>
-      <c r="E564"/>
-    </row>
-    <row r="565" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E564">
+        <v>1</v>
+      </c>
+      <c r="F564" t="s">
+        <v>14</v>
+      </c>
+      <c r="G564" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A565" s="17"/>
-      <c r="B565"/>
-      <c r="C565" s="11"/>
+      <c r="B565" t="s">
+        <v>628</v>
+      </c>
+      <c r="C565">
+        <v>22800</v>
+      </c>
       <c r="D565"/>
-      <c r="E565"/>
-    </row>
-    <row r="566" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E565">
+        <v>1</v>
+      </c>
+      <c r="F565" t="s">
+        <v>14</v>
+      </c>
+      <c r="G565" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A566" s="17"/>
-      <c r="B566"/>
-      <c r="C566" s="11"/>
+      <c r="B566" t="s">
+        <v>629</v>
+      </c>
+      <c r="C566">
+        <v>22800</v>
+      </c>
       <c r="D566"/>
-      <c r="E566"/>
-    </row>
-    <row r="567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E566">
+        <v>1</v>
+      </c>
+      <c r="F566" t="s">
+        <v>14</v>
+      </c>
+      <c r="G566" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A567" s="17"/>
-      <c r="B567"/>
-      <c r="C567" s="11"/>
+      <c r="B567" t="s">
+        <v>630</v>
+      </c>
+      <c r="C567">
+        <v>26800</v>
+      </c>
       <c r="D567"/>
-      <c r="E567"/>
-    </row>
-    <row r="568" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E567">
+        <v>1</v>
+      </c>
+      <c r="F567" t="s">
+        <v>14</v>
+      </c>
+      <c r="G567" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A568" s="17"/>
-      <c r="B568"/>
-      <c r="C568" s="11"/>
+      <c r="B568" t="s">
+        <v>631</v>
+      </c>
+      <c r="C568">
+        <v>28800</v>
+      </c>
       <c r="D568"/>
-      <c r="E568"/>
-    </row>
-    <row r="569" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E568">
+        <v>1</v>
+      </c>
+      <c r="F568" t="s">
+        <v>14</v>
+      </c>
+      <c r="G568" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A569" s="17"/>
-      <c r="B569"/>
-      <c r="C569" s="11"/>
+      <c r="B569" t="s">
+        <v>632</v>
+      </c>
+      <c r="C569">
+        <v>39800</v>
+      </c>
       <c r="D569"/>
-      <c r="E569"/>
-    </row>
-    <row r="570" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E569">
+        <v>1</v>
+      </c>
+      <c r="F569" t="s">
+        <v>14</v>
+      </c>
+      <c r="G569" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="570" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A570" s="17"/>
-      <c r="B570"/>
-      <c r="C570" s="11"/>
+      <c r="B570" t="s">
+        <v>633</v>
+      </c>
+      <c r="C570">
+        <v>29800</v>
+      </c>
       <c r="D570"/>
-      <c r="E570"/>
-    </row>
-    <row r="571" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E570">
+        <v>1</v>
+      </c>
+      <c r="F570" t="s">
+        <v>14</v>
+      </c>
+      <c r="G570" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A571" s="17"/>
-      <c r="B571"/>
-      <c r="C571" s="11"/>
+      <c r="B571" t="s">
+        <v>634</v>
+      </c>
+      <c r="C571">
+        <v>32800</v>
+      </c>
       <c r="D571"/>
-      <c r="E571"/>
-    </row>
-    <row r="572" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E571">
+        <v>1</v>
+      </c>
+      <c r="F571" t="s">
+        <v>14</v>
+      </c>
+      <c r="G571" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A572" s="17"/>
-      <c r="B572"/>
-      <c r="C572" s="11"/>
+      <c r="B572" t="s">
+        <v>635</v>
+      </c>
+      <c r="C572">
+        <v>8800</v>
+      </c>
       <c r="D572"/>
-      <c r="E572"/>
-    </row>
-    <row r="573" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E572">
+        <v>1</v>
+      </c>
+      <c r="F572" t="s">
+        <v>14</v>
+      </c>
+      <c r="G572" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A573" s="17"/>
-      <c r="B573"/>
-      <c r="C573" s="11"/>
+      <c r="B573" t="s">
+        <v>636</v>
+      </c>
+      <c r="C573">
+        <v>39800</v>
+      </c>
       <c r="D573"/>
-      <c r="E573"/>
-    </row>
-    <row r="574" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E573">
+        <v>1</v>
+      </c>
+      <c r="F573" t="s">
+        <v>14</v>
+      </c>
+      <c r="G573" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A574" s="17"/>
-      <c r="B574"/>
-      <c r="C574" s="11"/>
+      <c r="B574" t="s">
+        <v>637</v>
+      </c>
+      <c r="C574">
+        <v>25800</v>
+      </c>
       <c r="D574"/>
-      <c r="E574"/>
-    </row>
-    <row r="575" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E574">
+        <v>1</v>
+      </c>
+      <c r="F574" t="s">
+        <v>14</v>
+      </c>
+      <c r="G574" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="575" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A575" s="17"/>
-      <c r="B575"/>
-      <c r="C575" s="11"/>
+      <c r="B575" t="s">
+        <v>638</v>
+      </c>
+      <c r="C575">
+        <v>25800</v>
+      </c>
       <c r="D575"/>
-      <c r="E575"/>
-    </row>
-    <row r="576" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E575">
+        <v>1</v>
+      </c>
+      <c r="F575" t="s">
+        <v>14</v>
+      </c>
+      <c r="G575" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="576" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A576" s="17"/>
-      <c r="B576"/>
-      <c r="C576" s="11"/>
+      <c r="B576" t="s">
+        <v>639</v>
+      </c>
+      <c r="C576">
+        <v>19800</v>
+      </c>
       <c r="D576"/>
-      <c r="E576"/>
-    </row>
-    <row r="577" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E576">
+        <v>1</v>
+      </c>
+      <c r="F576" t="s">
+        <v>14</v>
+      </c>
+      <c r="G576" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="577" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A577" s="17"/>
-      <c r="B577"/>
-      <c r="C577" s="11"/>
+      <c r="B577" t="s">
+        <v>640</v>
+      </c>
+      <c r="C577">
+        <v>25800</v>
+      </c>
       <c r="D577"/>
-      <c r="E577"/>
-    </row>
-    <row r="578" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E577">
+        <v>1</v>
+      </c>
+      <c r="F577" t="s">
+        <v>14</v>
+      </c>
+      <c r="G577" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="578" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A578" s="17"/>
-      <c r="B578"/>
-      <c r="C578" s="11"/>
+      <c r="B578" t="s">
+        <v>641</v>
+      </c>
+      <c r="C578">
+        <v>39800</v>
+      </c>
       <c r="D578"/>
-      <c r="E578"/>
-    </row>
-    <row r="579" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E578">
+        <v>1</v>
+      </c>
+      <c r="F578" t="s">
+        <v>14</v>
+      </c>
+      <c r="G578" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="579" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A579" s="17"/>
-      <c r="B579"/>
-      <c r="C579" s="11"/>
+      <c r="B579" t="s">
+        <v>642</v>
+      </c>
+      <c r="C579">
+        <v>25800</v>
+      </c>
       <c r="D579"/>
-      <c r="E579"/>
-    </row>
-    <row r="580" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E579">
+        <v>1</v>
+      </c>
+      <c r="F579" t="s">
+        <v>14</v>
+      </c>
+      <c r="G579" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A580" s="17"/>
-      <c r="B580"/>
-      <c r="C580" s="11"/>
+      <c r="B580" t="s">
+        <v>643</v>
+      </c>
+      <c r="C580">
+        <v>25800</v>
+      </c>
       <c r="D580"/>
-      <c r="E580"/>
-    </row>
-    <row r="581" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E580">
+        <v>1</v>
+      </c>
+      <c r="F580" t="s">
+        <v>14</v>
+      </c>
+      <c r="G580" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="581" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A581" s="17"/>
-      <c r="B581"/>
-      <c r="C581" s="11"/>
+      <c r="B581" t="s">
+        <v>644</v>
+      </c>
+      <c r="C581">
+        <v>33800</v>
+      </c>
       <c r="D581"/>
-      <c r="E581"/>
-    </row>
-    <row r="582" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E581">
+        <v>1</v>
+      </c>
+      <c r="F581" t="s">
+        <v>14</v>
+      </c>
+      <c r="G581" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="582" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A582" s="17"/>
-      <c r="B582"/>
-      <c r="C582" s="11"/>
+      <c r="B582" t="s">
+        <v>645</v>
+      </c>
+      <c r="C582">
+        <v>28800</v>
+      </c>
       <c r="D582"/>
-      <c r="E582"/>
-    </row>
-    <row r="583" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E582">
+        <v>1</v>
+      </c>
+      <c r="F582" t="s">
+        <v>14</v>
+      </c>
+      <c r="G582" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="583" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A583" s="17"/>
-      <c r="B583"/>
-      <c r="C583" s="11"/>
+      <c r="B583" t="s">
+        <v>646</v>
+      </c>
+      <c r="C583">
+        <v>29800</v>
+      </c>
       <c r="D583"/>
-      <c r="E583"/>
-    </row>
-    <row r="584" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E583">
+        <v>1</v>
+      </c>
+      <c r="F583" t="s">
+        <v>14</v>
+      </c>
+      <c r="G583" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="584" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A584" s="17"/>
-      <c r="B584"/>
-      <c r="C584" s="11"/>
+      <c r="B584" t="s">
+        <v>647</v>
+      </c>
+      <c r="C584">
+        <v>29800</v>
+      </c>
       <c r="D584"/>
-      <c r="E584"/>
-    </row>
-    <row r="585" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E584">
+        <v>1</v>
+      </c>
+      <c r="F584" t="s">
+        <v>14</v>
+      </c>
+      <c r="G584" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="585" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A585" s="17"/>
-      <c r="B585"/>
-      <c r="C585" s="11"/>
+      <c r="B585" t="s">
+        <v>648</v>
+      </c>
+      <c r="C585">
+        <v>43800</v>
+      </c>
       <c r="D585"/>
-      <c r="E585"/>
-    </row>
-    <row r="586" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E585">
+        <v>1</v>
+      </c>
+      <c r="F585" t="s">
+        <v>14</v>
+      </c>
+      <c r="G585" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="586" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A586" s="17"/>
-      <c r="B586"/>
-      <c r="C586" s="11"/>
+      <c r="B586" t="s">
+        <v>649</v>
+      </c>
+      <c r="C586">
+        <v>29800</v>
+      </c>
       <c r="D586"/>
-      <c r="E586"/>
-    </row>
-    <row r="587" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E586">
+        <v>1</v>
+      </c>
+      <c r="F586" t="s">
+        <v>14</v>
+      </c>
+      <c r="G586" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="587" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A587" s="17"/>
-      <c r="B587"/>
-      <c r="C587" s="11"/>
+      <c r="B587" t="s">
+        <v>650</v>
+      </c>
+      <c r="C587">
+        <v>32800</v>
+      </c>
       <c r="D587"/>
-      <c r="E587"/>
-    </row>
-    <row r="588" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E587">
+        <v>1</v>
+      </c>
+      <c r="F587" t="s">
+        <v>14</v>
+      </c>
+      <c r="G587" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="588" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A588" s="17"/>
-      <c r="B588"/>
-      <c r="C588" s="11"/>
+      <c r="B588" t="s">
+        <v>651</v>
+      </c>
+      <c r="C588">
+        <v>42800</v>
+      </c>
       <c r="D588"/>
-      <c r="E588"/>
-    </row>
-    <row r="589" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E588">
+        <v>1</v>
+      </c>
+      <c r="F588" t="s">
+        <v>14</v>
+      </c>
+      <c r="G588" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="589" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A589" s="17"/>
-      <c r="B589"/>
-      <c r="C589" s="11"/>
+      <c r="B589" t="s">
+        <v>652</v>
+      </c>
+      <c r="C589">
+        <v>43800</v>
+      </c>
       <c r="D589"/>
-      <c r="E589"/>
-    </row>
-    <row r="590" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E589">
+        <v>1</v>
+      </c>
+      <c r="F589" t="s">
+        <v>14</v>
+      </c>
+      <c r="G589" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="590" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A590" s="17"/>
-      <c r="B590"/>
-      <c r="C590" s="11"/>
+      <c r="B590" t="s">
+        <v>653</v>
+      </c>
+      <c r="C590">
+        <v>39800</v>
+      </c>
       <c r="D590"/>
-      <c r="E590"/>
-    </row>
-    <row r="591" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E590">
+        <v>1</v>
+      </c>
+      <c r="F590" t="s">
+        <v>14</v>
+      </c>
+      <c r="G590" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="591" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A591" s="17"/>
-      <c r="B591"/>
-      <c r="C591" s="11"/>
+      <c r="B591" t="s">
+        <v>654</v>
+      </c>
+      <c r="C591">
+        <v>29800</v>
+      </c>
       <c r="D591"/>
-      <c r="E591"/>
-    </row>
-    <row r="592" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E591">
+        <v>1</v>
+      </c>
+      <c r="F591" t="s">
+        <v>14</v>
+      </c>
+      <c r="G591" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="592" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A592" s="17"/>
-      <c r="B592"/>
-      <c r="C592" s="11"/>
+      <c r="B592" t="s">
+        <v>655</v>
+      </c>
+      <c r="C592">
+        <v>26800</v>
+      </c>
       <c r="D592"/>
-      <c r="E592"/>
-    </row>
-    <row r="593" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E592">
+        <v>1</v>
+      </c>
+      <c r="F592" t="s">
+        <v>14</v>
+      </c>
+      <c r="G592" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="593" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A593" s="17"/>
-      <c r="B593"/>
-      <c r="C593" s="11"/>
+      <c r="B593" t="s">
+        <v>656</v>
+      </c>
+      <c r="C593">
+        <v>44800</v>
+      </c>
       <c r="D593"/>
-      <c r="E593"/>
-    </row>
-    <row r="594" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E593">
+        <v>1</v>
+      </c>
+      <c r="F593" t="s">
+        <v>14</v>
+      </c>
+      <c r="G593" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="594" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A594" s="17"/>
-      <c r="B594"/>
-      <c r="C594" s="11"/>
+      <c r="B594" t="s">
+        <v>657</v>
+      </c>
+      <c r="C594">
+        <v>23800</v>
+      </c>
       <c r="D594"/>
-      <c r="E594"/>
-    </row>
-    <row r="595" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E594">
+        <v>1</v>
+      </c>
+      <c r="F594" t="s">
+        <v>14</v>
+      </c>
+      <c r="G594" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="595" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A595" s="17"/>
-      <c r="B595"/>
-      <c r="C595" s="11"/>
+      <c r="B595" t="s">
+        <v>658</v>
+      </c>
+      <c r="C595">
+        <v>27800</v>
+      </c>
       <c r="D595"/>
-      <c r="E595"/>
-    </row>
-    <row r="596" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E595">
+        <v>1</v>
+      </c>
+      <c r="F595" t="s">
+        <v>14</v>
+      </c>
+      <c r="G595" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596" s="17"/>
-      <c r="B596"/>
-      <c r="C596" s="11"/>
+      <c r="B596" t="s">
+        <v>659</v>
+      </c>
+      <c r="C596">
+        <v>27800</v>
+      </c>
       <c r="D596"/>
-      <c r="E596"/>
-    </row>
-    <row r="597" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E596">
+        <v>1</v>
+      </c>
+      <c r="F596" t="s">
+        <v>14</v>
+      </c>
+      <c r="G596" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="597" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A597" s="17"/>
-      <c r="B597"/>
-      <c r="C597" s="11"/>
+      <c r="B597" t="s">
+        <v>660</v>
+      </c>
+      <c r="C597">
+        <v>33800</v>
+      </c>
       <c r="D597"/>
-      <c r="E597"/>
-    </row>
-    <row r="598" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E597">
+        <v>1</v>
+      </c>
+      <c r="F597" t="s">
+        <v>14</v>
+      </c>
+      <c r="G597" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="598" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A598" s="17"/>
-      <c r="B598"/>
-      <c r="C598" s="11"/>
+      <c r="B598" t="s">
+        <v>661</v>
+      </c>
+      <c r="C598">
+        <v>34800</v>
+      </c>
       <c r="D598"/>
-      <c r="E598"/>
-    </row>
-    <row r="599" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E598">
+        <v>1</v>
+      </c>
+      <c r="F598" t="s">
+        <v>14</v>
+      </c>
+      <c r="G598" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="599" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A599" s="17"/>
-      <c r="B599"/>
-      <c r="C599" s="11"/>
+      <c r="B599" t="s">
+        <v>662</v>
+      </c>
+      <c r="C599">
+        <v>29800</v>
+      </c>
       <c r="D599"/>
-      <c r="E599"/>
-    </row>
-    <row r="600" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E599">
+        <v>1</v>
+      </c>
+      <c r="F599" t="s">
+        <v>14</v>
+      </c>
+      <c r="G599" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="600" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A600" s="17"/>
-      <c r="B600"/>
-      <c r="C600" s="11"/>
+      <c r="B600" t="s">
+        <v>663</v>
+      </c>
+      <c r="C600">
+        <v>41800</v>
+      </c>
       <c r="D600"/>
-      <c r="E600"/>
-    </row>
-    <row r="601" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E600">
+        <v>1</v>
+      </c>
+      <c r="F600" t="s">
+        <v>14</v>
+      </c>
+      <c r="G600" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="601" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A601" s="17"/>
-      <c r="B601"/>
-      <c r="C601" s="11"/>
+      <c r="B601" t="s">
+        <v>664</v>
+      </c>
+      <c r="C601">
+        <v>36800</v>
+      </c>
       <c r="D601"/>
-      <c r="E601"/>
-    </row>
-    <row r="602" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E601">
+        <v>1</v>
+      </c>
+      <c r="F601" t="s">
+        <v>14</v>
+      </c>
+      <c r="G601" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A602" s="17"/>
-      <c r="B602"/>
-      <c r="C602" s="11"/>
+      <c r="B602" t="s">
+        <v>665</v>
+      </c>
+      <c r="C602">
+        <v>30800</v>
+      </c>
       <c r="D602"/>
-      <c r="E602"/>
-    </row>
-    <row r="603" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E602">
+        <v>1</v>
+      </c>
+      <c r="F602" t="s">
+        <v>14</v>
+      </c>
+      <c r="G602" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A603" s="17"/>
-      <c r="B603"/>
-      <c r="C603" s="11"/>
+      <c r="B603" t="s">
+        <v>666</v>
+      </c>
+      <c r="C603">
+        <v>27800</v>
+      </c>
       <c r="D603"/>
-      <c r="E603"/>
-    </row>
-    <row r="604" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E603">
+        <v>1</v>
+      </c>
+      <c r="F603" t="s">
+        <v>14</v>
+      </c>
+      <c r="G603" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A604" s="17"/>
-      <c r="B604"/>
-      <c r="C604" s="11"/>
+      <c r="B604" t="s">
+        <v>667</v>
+      </c>
+      <c r="C604">
+        <v>30800</v>
+      </c>
       <c r="D604"/>
-      <c r="E604"/>
-    </row>
-    <row r="605" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E604">
+        <v>1</v>
+      </c>
+      <c r="F604" t="s">
+        <v>14</v>
+      </c>
+      <c r="G604" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="605" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A605" s="17"/>
-      <c r="B605"/>
-      <c r="C605" s="11"/>
+      <c r="B605" t="s">
+        <v>668</v>
+      </c>
+      <c r="C605">
+        <v>35800</v>
+      </c>
       <c r="D605"/>
-      <c r="E605"/>
-    </row>
-    <row r="606" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E605">
+        <v>1</v>
+      </c>
+      <c r="F605" t="s">
+        <v>14</v>
+      </c>
+      <c r="G605" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="606" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A606" s="17"/>
-      <c r="B606"/>
-      <c r="C606" s="11"/>
+      <c r="B606" t="s">
+        <v>669</v>
+      </c>
+      <c r="C606">
+        <v>33800</v>
+      </c>
       <c r="D606"/>
-      <c r="E606"/>
-    </row>
-    <row r="607" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E606">
+        <v>1</v>
+      </c>
+      <c r="F606" t="s">
+        <v>14</v>
+      </c>
+      <c r="G606" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="607" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A607" s="17"/>
-      <c r="B607"/>
-      <c r="C607" s="11"/>
+      <c r="B607" t="s">
+        <v>670</v>
+      </c>
+      <c r="C607">
+        <v>33800</v>
+      </c>
       <c r="D607"/>
-      <c r="E607"/>
-    </row>
-    <row r="608" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E607">
+        <v>1</v>
+      </c>
+      <c r="F607" t="s">
+        <v>14</v>
+      </c>
+      <c r="G607" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="608" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A608" s="17"/>
-      <c r="B608"/>
-      <c r="C608" s="11"/>
+      <c r="B608" t="s">
+        <v>671</v>
+      </c>
+      <c r="C608">
+        <v>21800</v>
+      </c>
       <c r="D608"/>
-      <c r="E608"/>
-    </row>
-    <row r="609" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E608">
+        <v>1</v>
+      </c>
+      <c r="F608" t="s">
+        <v>14</v>
+      </c>
+      <c r="G608" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="609" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A609" s="17"/>
-      <c r="B609"/>
-      <c r="C609" s="11"/>
+      <c r="B609" t="s">
+        <v>672</v>
+      </c>
+      <c r="C609">
+        <v>18800</v>
+      </c>
       <c r="D609"/>
-      <c r="E609"/>
-    </row>
-    <row r="610" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E609">
+        <v>1</v>
+      </c>
+      <c r="F609" t="s">
+        <v>14</v>
+      </c>
+      <c r="G609" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="610" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A610" s="17"/>
-      <c r="B610"/>
-      <c r="C610" s="11"/>
+      <c r="B610" t="s">
+        <v>630</v>
+      </c>
+      <c r="C610">
+        <v>28800</v>
+      </c>
       <c r="D610"/>
-      <c r="E610"/>
-    </row>
-    <row r="611" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E610">
+        <v>1</v>
+      </c>
+      <c r="F610" t="s">
+        <v>14</v>
+      </c>
+      <c r="G610" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="611" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A611" s="17"/>
-      <c r="B611"/>
-      <c r="C611" s="11"/>
+      <c r="B611" t="s">
+        <v>673</v>
+      </c>
+      <c r="C611">
+        <v>23800</v>
+      </c>
       <c r="D611"/>
-      <c r="E611"/>
-    </row>
-    <row r="612" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E611">
+        <v>1</v>
+      </c>
+      <c r="F611" t="s">
+        <v>14</v>
+      </c>
+      <c r="G611" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="612" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A612" s="17"/>
-      <c r="B612"/>
-      <c r="C612" s="11"/>
+      <c r="B612" t="s">
+        <v>674</v>
+      </c>
+      <c r="C612">
+        <v>23800</v>
+      </c>
       <c r="D612"/>
-      <c r="E612"/>
-    </row>
-    <row r="613" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E612">
+        <v>1</v>
+      </c>
+      <c r="F612" t="s">
+        <v>14</v>
+      </c>
+      <c r="G612" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="613" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A613" s="17"/>
-      <c r="B613"/>
-      <c r="C613" s="11"/>
+      <c r="B613" t="s">
+        <v>675</v>
+      </c>
+      <c r="C613">
+        <v>26800</v>
+      </c>
       <c r="D613"/>
-      <c r="E613"/>
-    </row>
-    <row r="614" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E613">
+        <v>1</v>
+      </c>
+      <c r="F613" t="s">
+        <v>14</v>
+      </c>
+      <c r="G613" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="614" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A614" s="17"/>
-      <c r="B614"/>
-      <c r="C614" s="11"/>
+      <c r="B614" t="s">
+        <v>676</v>
+      </c>
+      <c r="C614">
+        <v>25800</v>
+      </c>
       <c r="D614"/>
-      <c r="E614"/>
-    </row>
-    <row r="615" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E614">
+        <v>1</v>
+      </c>
+      <c r="F614" t="s">
+        <v>14</v>
+      </c>
+      <c r="G614" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="615" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A615" s="17"/>
-      <c r="B615"/>
-      <c r="C615" s="11"/>
+      <c r="B615" t="s">
+        <v>677</v>
+      </c>
+      <c r="C615">
+        <v>16800</v>
+      </c>
       <c r="D615"/>
-      <c r="E615"/>
-    </row>
-    <row r="616" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E615">
+        <v>1</v>
+      </c>
+      <c r="F615" t="s">
+        <v>14</v>
+      </c>
+      <c r="G615" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="616" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A616" s="17"/>
-      <c r="B616"/>
-      <c r="C616" s="11"/>
+      <c r="B616" t="s">
+        <v>678</v>
+      </c>
+      <c r="C616">
+        <v>25800</v>
+      </c>
       <c r="D616"/>
-      <c r="E616"/>
-    </row>
-    <row r="617" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E616">
+        <v>1</v>
+      </c>
+      <c r="F616" t="s">
+        <v>14</v>
+      </c>
+      <c r="G616" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="617" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A617" s="17"/>
-      <c r="B617"/>
-      <c r="C617" s="11"/>
+      <c r="B617" t="s">
+        <v>679</v>
+      </c>
+      <c r="C617">
+        <v>16800</v>
+      </c>
       <c r="D617"/>
-      <c r="E617"/>
-    </row>
-    <row r="618" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E617">
+        <v>1</v>
+      </c>
+      <c r="F617" t="s">
+        <v>14</v>
+      </c>
+      <c r="G617" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="618" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A618" s="17"/>
-      <c r="B618"/>
-      <c r="C618" s="11"/>
+      <c r="B618" t="s">
+        <v>680</v>
+      </c>
+      <c r="C618">
+        <v>53800</v>
+      </c>
       <c r="D618"/>
-      <c r="E618"/>
-    </row>
-    <row r="619" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E618">
+        <v>1</v>
+      </c>
+      <c r="F618" t="s">
+        <v>14</v>
+      </c>
+      <c r="G618" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="619" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A619" s="17"/>
-      <c r="B619"/>
-      <c r="C619" s="11"/>
+      <c r="B619" t="s">
+        <v>681</v>
+      </c>
+      <c r="C619">
+        <v>53800</v>
+      </c>
       <c r="D619"/>
-      <c r="E619"/>
-    </row>
-    <row r="620" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E619">
+        <v>1</v>
+      </c>
+      <c r="F619" t="s">
+        <v>14</v>
+      </c>
+      <c r="G619" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="620" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A620" s="17"/>
-      <c r="B620"/>
-      <c r="C620" s="11"/>
+      <c r="B620" t="s">
+        <v>682</v>
+      </c>
+      <c r="C620">
+        <v>21800</v>
+      </c>
       <c r="D620"/>
-      <c r="E620"/>
-    </row>
-    <row r="621" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E620">
+        <v>1</v>
+      </c>
+      <c r="F620" t="s">
+        <v>14</v>
+      </c>
+      <c r="G620" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="621" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A621" s="17"/>
-      <c r="B621"/>
-      <c r="C621" s="11"/>
+      <c r="B621" t="s">
+        <v>683</v>
+      </c>
+      <c r="C621">
+        <v>22800</v>
+      </c>
       <c r="D621"/>
-      <c r="E621"/>
-    </row>
-    <row r="622" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E621">
+        <v>1</v>
+      </c>
+      <c r="F621" t="s">
+        <v>14</v>
+      </c>
+      <c r="G621" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="622" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A622" s="17"/>
-      <c r="B622"/>
-      <c r="C622" s="11"/>
+      <c r="B622" t="s">
+        <v>684</v>
+      </c>
+      <c r="C622">
+        <v>27800</v>
+      </c>
       <c r="D622"/>
-      <c r="E622"/>
-    </row>
-    <row r="623" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E622">
+        <v>1</v>
+      </c>
+      <c r="F622" t="s">
+        <v>14</v>
+      </c>
+      <c r="G622" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="623" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A623" s="17"/>
-      <c r="B623"/>
-      <c r="C623" s="11"/>
+      <c r="B623" t="s">
+        <v>685</v>
+      </c>
+      <c r="C623">
+        <v>29800</v>
+      </c>
       <c r="D623"/>
-      <c r="E623"/>
-    </row>
-    <row r="624" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E623">
+        <v>1</v>
+      </c>
+      <c r="F623" t="s">
+        <v>14</v>
+      </c>
+      <c r="G623" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="624" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A624" s="17"/>
-      <c r="B624"/>
-      <c r="C624" s="11"/>
+      <c r="B624" s="29" t="s">
+        <v>697</v>
+      </c>
+      <c r="C624">
+        <v>25800</v>
+      </c>
       <c r="D624"/>
-      <c r="E624"/>
-    </row>
-    <row r="625" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E624">
+        <v>1</v>
+      </c>
+      <c r="F624" t="s">
+        <v>14</v>
+      </c>
+      <c r="G624" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="625" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A625" s="17"/>
-      <c r="B625"/>
-      <c r="C625" s="11"/>
+      <c r="B625" s="29" t="s">
+        <v>698</v>
+      </c>
+      <c r="C625">
+        <v>25800</v>
+      </c>
       <c r="D625"/>
-      <c r="E625"/>
-    </row>
-    <row r="626" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E625">
+        <v>1</v>
+      </c>
+      <c r="F625" t="s">
+        <v>14</v>
+      </c>
+      <c r="G625" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="626" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A626" s="17"/>
-      <c r="B626"/>
-      <c r="C626" s="11"/>
+      <c r="B626" s="29" t="s">
+        <v>699</v>
+      </c>
+      <c r="C626">
+        <v>25800</v>
+      </c>
       <c r="D626"/>
-      <c r="E626"/>
-    </row>
-    <row r="627" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E626">
+        <v>1</v>
+      </c>
+      <c r="F626" t="s">
+        <v>14</v>
+      </c>
+      <c r="G626" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="627" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A627" s="17"/>
-      <c r="B627"/>
-      <c r="C627" s="11"/>
+      <c r="B627" s="29" t="s">
+        <v>700</v>
+      </c>
+      <c r="C627">
+        <v>25800</v>
+      </c>
       <c r="D627"/>
-      <c r="E627"/>
-    </row>
-    <row r="628" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E627">
+        <v>1</v>
+      </c>
+      <c r="F627" t="s">
+        <v>14</v>
+      </c>
+      <c r="G627" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="628" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A628" s="17"/>
-      <c r="B628"/>
-      <c r="C628" s="11"/>
+      <c r="B628" t="s">
+        <v>686</v>
+      </c>
+      <c r="C628">
+        <v>26800</v>
+      </c>
       <c r="D628"/>
-      <c r="E628"/>
-    </row>
-    <row r="629" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E628">
+        <v>1</v>
+      </c>
+      <c r="F628" t="s">
+        <v>61</v>
+      </c>
+      <c r="G628" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="629" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A629" s="17"/>
-      <c r="B629"/>
-      <c r="C629" s="11"/>
+      <c r="B629" t="s">
+        <v>687</v>
+      </c>
+      <c r="C629">
+        <v>26800</v>
+      </c>
       <c r="D629"/>
-      <c r="E629"/>
-    </row>
-    <row r="630" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E629">
+        <v>1</v>
+      </c>
+      <c r="F629" t="s">
+        <v>61</v>
+      </c>
+      <c r="G629" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="630" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A630" s="17"/>
-      <c r="B630"/>
-      <c r="C630" s="11"/>
+      <c r="B630" t="s">
+        <v>688</v>
+      </c>
+      <c r="C630">
+        <v>26800</v>
+      </c>
       <c r="D630"/>
-      <c r="E630"/>
-    </row>
-    <row r="631" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E630">
+        <v>1</v>
+      </c>
+      <c r="F630" t="s">
+        <v>61</v>
+      </c>
+      <c r="G630" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="631" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A631" s="17"/>
-      <c r="B631"/>
-      <c r="C631" s="11"/>
+      <c r="B631" t="s">
+        <v>689</v>
+      </c>
+      <c r="C631">
+        <v>31800</v>
+      </c>
       <c r="D631"/>
-      <c r="E631"/>
-    </row>
-    <row r="632" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E631">
+        <v>2</v>
+      </c>
+      <c r="F631" t="s">
+        <v>61</v>
+      </c>
+      <c r="G631" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="632" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A632" s="17"/>
-      <c r="B632"/>
-      <c r="C632" s="11"/>
+      <c r="B632" t="s">
+        <v>690</v>
+      </c>
+      <c r="C632">
+        <v>26800</v>
+      </c>
       <c r="D632"/>
-      <c r="E632"/>
-    </row>
-    <row r="633" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E632">
+        <v>1</v>
+      </c>
+      <c r="F632" t="s">
+        <v>61</v>
+      </c>
+      <c r="G632" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633" s="17"/>
-      <c r="B633"/>
-      <c r="C633" s="11"/>
+      <c r="B633" t="s">
+        <v>691</v>
+      </c>
+      <c r="C633">
+        <v>8800</v>
+      </c>
       <c r="D633"/>
-      <c r="E633"/>
-    </row>
-    <row r="634" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E633">
+        <v>1</v>
+      </c>
+      <c r="F633" t="s">
+        <v>61</v>
+      </c>
+      <c r="G633" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="634" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A634" s="17"/>
-      <c r="B634"/>
-      <c r="C634" s="11"/>
+      <c r="B634" t="s">
+        <v>595</v>
+      </c>
+      <c r="C634">
+        <v>13800</v>
+      </c>
       <c r="D634"/>
-      <c r="E634"/>
-    </row>
-    <row r="635" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E634">
+        <v>1</v>
+      </c>
+      <c r="F634" t="s">
+        <v>61</v>
+      </c>
+      <c r="G634" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="635" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A635" s="17"/>
-      <c r="B635"/>
-      <c r="C635" s="11"/>
+      <c r="B635" t="s">
+        <v>692</v>
+      </c>
+      <c r="C635">
+        <v>13800</v>
+      </c>
       <c r="D635"/>
-      <c r="E635"/>
-    </row>
-    <row r="636" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E635">
+        <v>1</v>
+      </c>
+      <c r="F635" t="s">
+        <v>61</v>
+      </c>
+      <c r="G635" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="636" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A636" s="17"/>
-      <c r="B636"/>
-      <c r="C636" s="11"/>
+      <c r="B636" t="s">
+        <v>693</v>
+      </c>
+      <c r="C636">
+        <v>13800</v>
+      </c>
       <c r="D636"/>
-      <c r="E636"/>
-    </row>
-    <row r="637" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E636">
+        <v>1</v>
+      </c>
+      <c r="F636" t="s">
+        <v>61</v>
+      </c>
+      <c r="G636" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="637" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A637" s="17"/>
-      <c r="B637"/>
-      <c r="C637" s="11"/>
+      <c r="B637" t="s">
+        <v>694</v>
+      </c>
+      <c r="C637">
+        <v>14800</v>
+      </c>
       <c r="D637"/>
-      <c r="E637"/>
-    </row>
-    <row r="638" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E637">
+        <v>1</v>
+      </c>
+      <c r="F637" t="s">
+        <v>61</v>
+      </c>
+      <c r="G637" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="638" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A638" s="17"/>
-      <c r="B638"/>
-      <c r="C638" s="11"/>
+      <c r="B638" t="s">
+        <v>331</v>
+      </c>
+      <c r="C638">
+        <v>11800</v>
+      </c>
       <c r="D638"/>
-      <c r="E638"/>
-    </row>
-    <row r="639" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E638">
+        <v>1</v>
+      </c>
+      <c r="F638" t="s">
+        <v>61</v>
+      </c>
+      <c r="G638" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="639" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A639" s="17"/>
-      <c r="B639"/>
-      <c r="C639" s="11"/>
+      <c r="B639" t="s">
+        <v>695</v>
+      </c>
+      <c r="C639">
+        <v>11800</v>
+      </c>
       <c r="D639"/>
-      <c r="E639"/>
-    </row>
-    <row r="640" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E639">
+        <v>1</v>
+      </c>
+      <c r="F639" t="s">
+        <v>61</v>
+      </c>
+      <c r="G639" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="640" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A640" s="17"/>
-      <c r="B640"/>
-      <c r="C640" s="11"/>
+      <c r="B640" t="s">
+        <v>349</v>
+      </c>
+      <c r="C640">
+        <v>7800</v>
+      </c>
       <c r="D640"/>
-      <c r="E640"/>
-    </row>
-    <row r="641" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E640">
+        <v>1</v>
+      </c>
+      <c r="F640" t="s">
+        <v>61</v>
+      </c>
+      <c r="G640" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="641" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A641" s="17"/>
-      <c r="B641"/>
-      <c r="C641" s="11"/>
+      <c r="B641" t="s">
+        <v>696</v>
+      </c>
+      <c r="C641">
+        <v>8800</v>
+      </c>
       <c r="D641"/>
-      <c r="E641"/>
-    </row>
-    <row r="642" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A642" s="17"/>
-      <c r="B642"/>
-      <c r="C642" s="11"/>
+      <c r="E641">
+        <v>1</v>
+      </c>
+      <c r="F641" t="s">
+        <v>61</v>
+      </c>
+      <c r="G641" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="642" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A642" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B642" t="s">
+        <v>69</v>
+      </c>
+      <c r="C642">
+        <v>9500</v>
+      </c>
       <c r="D642"/>
-      <c r="E642"/>
-    </row>
-    <row r="643" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E642">
+        <v>1</v>
+      </c>
+      <c r="F642" t="s">
+        <v>14</v>
+      </c>
+      <c r="G642" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="643" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A643" s="17"/>
-      <c r="B643"/>
-      <c r="C643" s="11"/>
+      <c r="B643" t="s">
+        <v>701</v>
+      </c>
+      <c r="C643">
+        <v>9500</v>
+      </c>
       <c r="D643"/>
-      <c r="E643"/>
-    </row>
-    <row r="644" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E643">
+        <v>1</v>
+      </c>
+      <c r="F643" t="s">
+        <v>14</v>
+      </c>
+      <c r="G643" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="644" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A644" s="17"/>
-      <c r="B644"/>
-      <c r="C644" s="11"/>
+      <c r="B644" t="s">
+        <v>597</v>
+      </c>
+      <c r="C644">
+        <v>6000</v>
+      </c>
       <c r="D644"/>
-      <c r="E644"/>
-    </row>
-    <row r="645" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E644">
+        <v>1</v>
+      </c>
+      <c r="F644" t="s">
+        <v>61</v>
+      </c>
+      <c r="G644" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="645" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A645" s="17"/>
-      <c r="B645"/>
-      <c r="C645" s="11"/>
+      <c r="B645" t="s">
+        <v>702</v>
+      </c>
+      <c r="C645">
+        <v>5000</v>
+      </c>
       <c r="D645"/>
-      <c r="E645"/>
-    </row>
-    <row r="646" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E645">
+        <v>1</v>
+      </c>
+      <c r="F645" t="s">
+        <v>61</v>
+      </c>
+      <c r="G645" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="646" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A646" s="17"/>
-      <c r="B646"/>
-      <c r="C646" s="11"/>
+      <c r="B646" t="s">
+        <v>703</v>
+      </c>
+      <c r="C646">
+        <v>8000</v>
+      </c>
       <c r="D646"/>
-      <c r="E646"/>
-    </row>
-    <row r="647" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E646">
+        <v>1</v>
+      </c>
+      <c r="F646" t="s">
+        <v>61</v>
+      </c>
+      <c r="G646" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="647" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A647" s="17"/>
-      <c r="B647"/>
-      <c r="C647" s="11"/>
+      <c r="B647" t="s">
+        <v>704</v>
+      </c>
+      <c r="C647">
+        <v>8000</v>
+      </c>
       <c r="D647"/>
-      <c r="E647"/>
-    </row>
-    <row r="648" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E647">
+        <v>1</v>
+      </c>
+      <c r="F647" t="s">
+        <v>61</v>
+      </c>
+      <c r="G647" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="648" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A648" s="17"/>
-      <c r="B648"/>
-      <c r="C648" s="11"/>
+      <c r="B648" t="s">
+        <v>705</v>
+      </c>
+      <c r="C648">
+        <v>9000</v>
+      </c>
       <c r="D648"/>
-      <c r="E648"/>
-    </row>
-    <row r="649" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A649" s="17"/>
-      <c r="B649"/>
-      <c r="C649" s="11"/>
+      <c r="E648">
+        <v>1</v>
+      </c>
+      <c r="F648" t="s">
+        <v>61</v>
+      </c>
+      <c r="G648" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="649" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A649" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B649" t="s">
+        <v>706</v>
+      </c>
+      <c r="C649">
+        <v>31818</v>
+      </c>
       <c r="D649"/>
-      <c r="E649"/>
-    </row>
-    <row r="650" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E649">
+        <v>1</v>
+      </c>
+      <c r="F649" t="s">
+        <v>14</v>
+      </c>
+      <c r="G649" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="650" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A650" s="17"/>
-      <c r="B650"/>
-      <c r="C650" s="11"/>
+      <c r="B650" t="s">
+        <v>707</v>
+      </c>
+      <c r="C650">
+        <v>39090</v>
+      </c>
       <c r="D650"/>
-      <c r="E650"/>
-    </row>
-    <row r="651" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E650">
+        <v>1</v>
+      </c>
+      <c r="F650" t="s">
+        <v>14</v>
+      </c>
+      <c r="G650" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="651" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A651" s="17"/>
-      <c r="B651"/>
-      <c r="C651" s="11"/>
+      <c r="B651" t="s">
+        <v>708</v>
+      </c>
+      <c r="C651">
+        <v>31818</v>
+      </c>
       <c r="D651"/>
-      <c r="E651"/>
-    </row>
-    <row r="652" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E651">
+        <v>1</v>
+      </c>
+      <c r="F651" t="s">
+        <v>14</v>
+      </c>
+      <c r="G651" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="652" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A652" s="17"/>
-      <c r="B652"/>
-      <c r="C652" s="11"/>
+      <c r="B652" t="s">
+        <v>709</v>
+      </c>
+      <c r="C652">
+        <v>39090</v>
+      </c>
       <c r="D652"/>
-      <c r="E652"/>
-    </row>
-    <row r="653" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E652">
+        <v>1</v>
+      </c>
+      <c r="F652" t="s">
+        <v>14</v>
+      </c>
+      <c r="G652" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="653" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A653" s="17"/>
-      <c r="B653"/>
-      <c r="C653" s="11"/>
+      <c r="B653" t="s">
+        <v>710</v>
+      </c>
+      <c r="C653">
+        <v>35454</v>
+      </c>
       <c r="D653"/>
-      <c r="E653"/>
-    </row>
-    <row r="654" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E653">
+        <v>1</v>
+      </c>
+      <c r="F653" t="s">
+        <v>14</v>
+      </c>
+      <c r="G653" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" s="17"/>
-      <c r="B654"/>
-      <c r="C654" s="11"/>
+      <c r="B654" t="s">
+        <v>711</v>
+      </c>
+      <c r="C654">
+        <v>42727</v>
+      </c>
       <c r="D654"/>
-      <c r="E654"/>
-    </row>
-    <row r="655" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E654">
+        <v>1</v>
+      </c>
+      <c r="F654" t="s">
+        <v>14</v>
+      </c>
+      <c r="G654" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="655" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A655" s="17"/>
-      <c r="B655"/>
-      <c r="C655" s="11"/>
+      <c r="B655" t="s">
+        <v>712</v>
+      </c>
+      <c r="C655">
+        <v>35454</v>
+      </c>
       <c r="D655"/>
-      <c r="E655"/>
-    </row>
-    <row r="656" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E655">
+        <v>1</v>
+      </c>
+      <c r="F655" t="s">
+        <v>14</v>
+      </c>
+      <c r="G655" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="656" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A656" s="17"/>
-      <c r="B656"/>
-      <c r="C656" s="11"/>
+      <c r="B656" t="s">
+        <v>713</v>
+      </c>
+      <c r="C656">
+        <v>42727</v>
+      </c>
       <c r="D656"/>
-      <c r="E656"/>
-    </row>
-    <row r="657" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E656">
+        <v>1</v>
+      </c>
+      <c r="F656" t="s">
+        <v>14</v>
+      </c>
+      <c r="G656" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A657" s="17"/>
-      <c r="B657"/>
-      <c r="C657" s="11"/>
+      <c r="B657" t="s">
+        <v>714</v>
+      </c>
+      <c r="C657">
+        <v>35454</v>
+      </c>
       <c r="D657"/>
-      <c r="E657"/>
-    </row>
-    <row r="658" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E657">
+        <v>1</v>
+      </c>
+      <c r="F657" t="s">
+        <v>14</v>
+      </c>
+      <c r="G657" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" s="17"/>
-      <c r="B658"/>
-      <c r="C658" s="11"/>
+      <c r="B658" t="s">
+        <v>715</v>
+      </c>
+      <c r="C658">
+        <v>42727</v>
+      </c>
       <c r="D658"/>
-      <c r="E658"/>
-    </row>
-    <row r="659" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E658">
+        <v>1</v>
+      </c>
+      <c r="F658" t="s">
+        <v>14</v>
+      </c>
+      <c r="G658" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="659" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A659" s="17"/>
-      <c r="B659"/>
-      <c r="C659" s="11"/>
+      <c r="B659" t="s">
+        <v>716</v>
+      </c>
+      <c r="C659">
+        <v>35454</v>
+      </c>
       <c r="D659"/>
-      <c r="E659"/>
-    </row>
-    <row r="660" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E659">
+        <v>1</v>
+      </c>
+      <c r="F659" t="s">
+        <v>14</v>
+      </c>
+      <c r="G659" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="660" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A660" s="17"/>
-      <c r="B660"/>
-      <c r="C660" s="11"/>
+      <c r="B660" t="s">
+        <v>717</v>
+      </c>
+      <c r="C660">
+        <v>42727</v>
+      </c>
       <c r="D660"/>
-      <c r="E660"/>
-    </row>
-    <row r="661" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E660">
+        <v>1</v>
+      </c>
+      <c r="F660" t="s">
+        <v>14</v>
+      </c>
+      <c r="G660" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="661" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A661" s="17"/>
-      <c r="B661"/>
-      <c r="C661" s="11"/>
+      <c r="B661" t="s">
+        <v>718</v>
+      </c>
+      <c r="C661">
+        <v>35454</v>
+      </c>
       <c r="D661"/>
-      <c r="E661"/>
-    </row>
-    <row r="662" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E661">
+        <v>1</v>
+      </c>
+      <c r="F661" t="s">
+        <v>14</v>
+      </c>
+      <c r="G661" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="662" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A662" s="17"/>
-      <c r="B662"/>
-      <c r="C662" s="11"/>
+      <c r="B662" t="s">
+        <v>719</v>
+      </c>
+      <c r="C662">
+        <v>42727</v>
+      </c>
       <c r="D662"/>
-      <c r="E662"/>
-    </row>
-    <row r="663" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E662">
+        <v>1</v>
+      </c>
+      <c r="F662" t="s">
+        <v>14</v>
+      </c>
+      <c r="G662" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="663" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A663" s="17"/>
-      <c r="B663"/>
-      <c r="C663" s="11"/>
+      <c r="B663" s="33" t="s">
+        <v>720</v>
+      </c>
+      <c r="C663" s="31"/>
       <c r="D663"/>
-      <c r="E663"/>
-    </row>
-    <row r="664" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E663" s="31"/>
+      <c r="F663" s="31"/>
+    </row>
+    <row r="664" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A664" s="17"/>
-      <c r="B664"/>
-      <c r="C664" s="11"/>
+      <c r="B664" s="31" t="s">
+        <v>721</v>
+      </c>
+      <c r="C664" s="31">
+        <v>5454</v>
+      </c>
       <c r="D664"/>
-      <c r="E664"/>
-    </row>
-    <row r="665" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E664" s="31">
+        <v>1</v>
+      </c>
+      <c r="F664" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G664" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="665" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A665" s="17"/>
-      <c r="B665"/>
-      <c r="C665" s="11"/>
+      <c r="B665" s="31" t="s">
+        <v>722</v>
+      </c>
+      <c r="C665" s="31">
+        <v>5454</v>
+      </c>
       <c r="D665"/>
-      <c r="E665"/>
-    </row>
-    <row r="666" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E665" s="31">
+        <v>1</v>
+      </c>
+      <c r="F665" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G665" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="666" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A666" s="17"/>
-      <c r="B666"/>
-      <c r="C666" s="11"/>
+      <c r="B666" s="31" t="s">
+        <v>723</v>
+      </c>
+      <c r="C666" s="31">
+        <v>5454</v>
+      </c>
       <c r="D666"/>
-      <c r="E666"/>
-    </row>
-    <row r="667" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E666" s="31">
+        <v>1</v>
+      </c>
+      <c r="F666" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G666" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="667" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A667" s="17"/>
-      <c r="B667"/>
-      <c r="C667" s="11"/>
+      <c r="B667" s="31" t="s">
+        <v>724</v>
+      </c>
+      <c r="C667" s="31">
+        <v>5454</v>
+      </c>
       <c r="D667"/>
-      <c r="E667"/>
-    </row>
-    <row r="668" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E667" s="31">
+        <v>1</v>
+      </c>
+      <c r="F667" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G667" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668" s="17"/>
-      <c r="B668"/>
-      <c r="C668" s="11"/>
+      <c r="B668" s="33" t="s">
+        <v>740</v>
+      </c>
+      <c r="C668" s="32">
+        <v>44545</v>
+      </c>
       <c r="D668"/>
-      <c r="E668"/>
-    </row>
-    <row r="669" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E668" s="32">
+        <v>1</v>
+      </c>
+      <c r="F668" t="s">
+        <v>14</v>
+      </c>
+      <c r="G668" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669" s="17"/>
-      <c r="B669"/>
-      <c r="C669" s="11"/>
+      <c r="B669" s="33" t="s">
+        <v>741</v>
+      </c>
+      <c r="C669" s="32">
+        <v>44545</v>
+      </c>
       <c r="D669"/>
-      <c r="E669"/>
-    </row>
-    <row r="670" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E669" s="32">
+        <v>1</v>
+      </c>
+      <c r="F669" t="s">
+        <v>14</v>
+      </c>
+      <c r="G669" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670" s="17"/>
-      <c r="B670"/>
-      <c r="C670" s="11"/>
+      <c r="B670" s="33" t="s">
+        <v>742</v>
+      </c>
+      <c r="C670" s="32">
+        <v>44545</v>
+      </c>
       <c r="D670"/>
-      <c r="E670"/>
-    </row>
-    <row r="671" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E670" s="32">
+        <v>1</v>
+      </c>
+      <c r="F670" t="s">
+        <v>14</v>
+      </c>
+      <c r="G670" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A671" s="17"/>
-      <c r="B671"/>
-      <c r="C671" s="11"/>
+      <c r="B671" s="33" t="s">
+        <v>743</v>
+      </c>
+      <c r="C671" s="32">
+        <v>44545</v>
+      </c>
       <c r="D671"/>
-      <c r="E671"/>
-    </row>
-    <row r="672" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E671" s="32">
+        <v>1</v>
+      </c>
+      <c r="F671" t="s">
+        <v>14</v>
+      </c>
+      <c r="G671" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672" s="17"/>
-      <c r="B672"/>
-      <c r="C672" s="11"/>
+      <c r="B672" s="34" t="s">
+        <v>744</v>
+      </c>
+      <c r="C672" s="31">
+        <v>20909</v>
+      </c>
       <c r="D672"/>
-      <c r="E672"/>
-    </row>
-    <row r="673" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E672" s="32">
+        <v>1</v>
+      </c>
+      <c r="F672" t="s">
+        <v>14</v>
+      </c>
+      <c r="G672" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="673" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A673" s="17"/>
-      <c r="B673"/>
-      <c r="C673" s="11"/>
+      <c r="B673" s="32" t="s">
+        <v>725</v>
+      </c>
+      <c r="C673" s="31">
+        <v>31818</v>
+      </c>
       <c r="D673"/>
-      <c r="E673"/>
-    </row>
-    <row r="674" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E673" s="32">
+        <v>1</v>
+      </c>
+      <c r="F673" t="s">
+        <v>14</v>
+      </c>
+      <c r="G673" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674" s="17"/>
-      <c r="B674"/>
-      <c r="C674" s="11"/>
+      <c r="B674" s="32" t="s">
+        <v>726</v>
+      </c>
+      <c r="C674" s="31">
+        <v>39090</v>
+      </c>
       <c r="D674"/>
-      <c r="E674"/>
-    </row>
-    <row r="675" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E674" s="32">
+        <v>1</v>
+      </c>
+      <c r="F674" t="s">
+        <v>14</v>
+      </c>
+      <c r="G674" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675" s="17"/>
-      <c r="B675"/>
-      <c r="C675" s="11"/>
+      <c r="B675" s="32" t="s">
+        <v>727</v>
+      </c>
+      <c r="C675" s="31">
+        <v>27272</v>
+      </c>
       <c r="D675"/>
-      <c r="E675"/>
-    </row>
-    <row r="676" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E675" s="32">
+        <v>1</v>
+      </c>
+      <c r="F675" t="s">
+        <v>14</v>
+      </c>
+      <c r="G675" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="676" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A676" s="17"/>
-      <c r="B676"/>
-      <c r="C676" s="11"/>
+      <c r="B676" s="32" t="s">
+        <v>728</v>
+      </c>
+      <c r="C676" s="31">
+        <v>32727</v>
+      </c>
       <c r="D676"/>
-      <c r="E676"/>
-    </row>
-    <row r="677" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E676" s="32">
+        <v>1</v>
+      </c>
+      <c r="F676" t="s">
+        <v>14</v>
+      </c>
+      <c r="G676" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" s="17"/>
-      <c r="B677"/>
-      <c r="C677" s="11"/>
+      <c r="B677" s="34" t="s">
+        <v>745</v>
+      </c>
+      <c r="C677" s="31">
+        <v>49090</v>
+      </c>
       <c r="D677"/>
-      <c r="E677"/>
-    </row>
-    <row r="678" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E677" s="32">
+        <v>1</v>
+      </c>
+      <c r="F677" t="s">
+        <v>14</v>
+      </c>
+      <c r="G677" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" s="17"/>
-      <c r="B678"/>
-      <c r="C678" s="11"/>
+      <c r="B678" s="32" t="s">
+        <v>729</v>
+      </c>
+      <c r="C678" s="32">
+        <v>26363</v>
+      </c>
       <c r="D678"/>
-      <c r="E678"/>
-    </row>
-    <row r="679" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E678" s="32">
+        <v>1</v>
+      </c>
+      <c r="F678" t="s">
+        <v>14</v>
+      </c>
+      <c r="G678" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" s="17"/>
-      <c r="B679"/>
-      <c r="C679" s="11"/>
+      <c r="B679" s="32" t="s">
+        <v>730</v>
+      </c>
+      <c r="C679" s="32">
+        <v>16363</v>
+      </c>
       <c r="D679"/>
-      <c r="E679"/>
-    </row>
-    <row r="680" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E679" s="32">
+        <v>1</v>
+      </c>
+      <c r="F679" t="s">
+        <v>14</v>
+      </c>
+      <c r="G679" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="680" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A680" s="17"/>
-      <c r="B680"/>
-      <c r="C680" s="11"/>
+      <c r="B680" s="32" t="s">
+        <v>731</v>
+      </c>
+      <c r="C680" s="32">
+        <v>26363</v>
+      </c>
       <c r="D680"/>
-      <c r="E680"/>
-    </row>
-    <row r="681" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E680" s="32">
+        <v>1</v>
+      </c>
+      <c r="F680" t="s">
+        <v>14</v>
+      </c>
+      <c r="G680" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="681" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A681" s="17"/>
-      <c r="B681"/>
-      <c r="C681" s="11"/>
+      <c r="B681" s="32" t="s">
+        <v>732</v>
+      </c>
+      <c r="C681" s="32">
+        <v>15454</v>
+      </c>
       <c r="D681"/>
-      <c r="E681"/>
-    </row>
-    <row r="682" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E681" s="32">
+        <v>1</v>
+      </c>
+      <c r="F681" t="s">
+        <v>14</v>
+      </c>
+      <c r="G681" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="682" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A682" s="17"/>
-      <c r="B682"/>
-      <c r="C682" s="11"/>
+      <c r="B682" s="32" t="s">
+        <v>733</v>
+      </c>
+      <c r="C682" s="32">
+        <v>15454</v>
+      </c>
       <c r="D682"/>
-      <c r="E682"/>
-    </row>
-    <row r="683" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E682" s="32">
+        <v>1</v>
+      </c>
+      <c r="F682" t="s">
+        <v>14</v>
+      </c>
+      <c r="G682" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="683" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A683" s="17"/>
-      <c r="B683"/>
-      <c r="C683" s="11"/>
+      <c r="B683" s="32" t="s">
+        <v>734</v>
+      </c>
+      <c r="C683" s="32">
+        <v>26363</v>
+      </c>
       <c r="D683"/>
-      <c r="E683"/>
-    </row>
-    <row r="684" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E683" s="32">
+        <v>1</v>
+      </c>
+      <c r="F683" t="s">
+        <v>14</v>
+      </c>
+      <c r="G683" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="684" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A684" s="17"/>
-      <c r="B684"/>
-      <c r="C684" s="11"/>
+      <c r="B684" s="32" t="s">
+        <v>735</v>
+      </c>
+      <c r="C684" s="32">
+        <v>16363</v>
+      </c>
       <c r="D684"/>
-      <c r="E684"/>
-    </row>
-    <row r="685" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E684" s="32">
+        <v>1</v>
+      </c>
+      <c r="F684" t="s">
+        <v>14</v>
+      </c>
+      <c r="G684" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="685" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A685" s="17"/>
-      <c r="B685"/>
-      <c r="C685" s="11"/>
+      <c r="B685" s="32" t="s">
+        <v>736</v>
+      </c>
+      <c r="C685" s="32">
+        <v>26363</v>
+      </c>
       <c r="D685"/>
-      <c r="E685"/>
-    </row>
-    <row r="686" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E685" s="32">
+        <v>1</v>
+      </c>
+      <c r="F685" t="s">
+        <v>14</v>
+      </c>
+      <c r="G685" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="686" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A686" s="17"/>
-      <c r="B686"/>
-      <c r="C686" s="11"/>
+      <c r="B686" s="32" t="s">
+        <v>737</v>
+      </c>
+      <c r="C686" s="32">
+        <v>22727</v>
+      </c>
       <c r="D686"/>
-      <c r="E686"/>
-    </row>
-    <row r="687" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E686" s="32">
+        <v>1</v>
+      </c>
+      <c r="F686" t="s">
+        <v>14</v>
+      </c>
+      <c r="G686" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="687" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A687" s="17"/>
-      <c r="B687"/>
-      <c r="C687" s="11"/>
+      <c r="B687" s="32" t="s">
+        <v>738</v>
+      </c>
+      <c r="C687" s="32">
+        <v>16363</v>
+      </c>
       <c r="D687"/>
-      <c r="E687"/>
-    </row>
-    <row r="688" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E687" s="32">
+        <v>1</v>
+      </c>
+      <c r="F687" t="s">
+        <v>14</v>
+      </c>
+      <c r="G687" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="688" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A688" s="17"/>
-      <c r="B688"/>
-      <c r="C688" s="11"/>
+      <c r="B688" s="32" t="s">
+        <v>739</v>
+      </c>
+      <c r="C688" s="32">
+        <v>9090</v>
+      </c>
       <c r="D688"/>
-      <c r="E688"/>
-    </row>
-    <row r="689" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E688" s="32">
+        <v>1</v>
+      </c>
+      <c r="F688" t="s">
+        <v>14</v>
+      </c>
+      <c r="G688" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="689" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A689" s="17"/>
-      <c r="B689"/>
-      <c r="C689" s="11"/>
+      <c r="B689" s="32"/>
+      <c r="C689" s="31"/>
       <c r="D689"/>
-      <c r="E689"/>
-    </row>
-    <row r="690" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E689" s="31"/>
+      <c r="F689" s="31"/>
+    </row>
+    <row r="690" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A690" s="17"/>
-      <c r="B690"/>
-      <c r="C690" s="11"/>
+      <c r="B690" s="4"/>
+      <c r="C690" s="30"/>
       <c r="D690"/>
-      <c r="E690"/>
-    </row>
-    <row r="691" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E690" s="32"/>
+      <c r="F690" s="32"/>
+    </row>
+    <row r="691" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A691" s="17"/>
-      <c r="B691"/>
-      <c r="C691" s="11"/>
+      <c r="B691" s="4"/>
+      <c r="C691" s="30"/>
       <c r="D691"/>
-      <c r="E691"/>
-    </row>
-    <row r="692" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E691" s="32"/>
+      <c r="F691" s="32"/>
+    </row>
+    <row r="692" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A692" s="17"/>
-      <c r="B692"/>
-      <c r="C692" s="11"/>
+      <c r="B692" s="4"/>
+      <c r="C692" s="30"/>
       <c r="D692"/>
-      <c r="E692"/>
-    </row>
-    <row r="693" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E692" s="32"/>
+      <c r="F692" s="32"/>
+    </row>
+    <row r="693" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A693" s="17"/>
-      <c r="B693"/>
-      <c r="C693" s="11"/>
+      <c r="B693" s="4"/>
+      <c r="C693" s="30"/>
       <c r="D693"/>
-      <c r="E693"/>
-    </row>
-    <row r="694" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E693" s="32"/>
+      <c r="F693" s="32"/>
+    </row>
+    <row r="694" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A694" s="17"/>
-      <c r="B694"/>
-      <c r="C694" s="11"/>
+      <c r="B694" s="4"/>
+      <c r="C694" s="30"/>
       <c r="D694"/>
-      <c r="E694"/>
-    </row>
-    <row r="695" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E694" s="32"/>
+      <c r="F694" s="32"/>
+    </row>
+    <row r="695" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A695" s="17"/>
-      <c r="B695"/>
-      <c r="C695" s="11"/>
+      <c r="B695" s="4"/>
+      <c r="C695" s="30"/>
       <c r="D695"/>
-      <c r="E695"/>
-    </row>
-    <row r="696" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E695" s="32"/>
+      <c r="F695" s="32"/>
+    </row>
+    <row r="696" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A696" s="17"/>
-      <c r="B696"/>
-      <c r="C696" s="11"/>
+      <c r="B696" s="4"/>
+      <c r="C696" s="30"/>
       <c r="D696"/>
-      <c r="E696"/>
-    </row>
-    <row r="697" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E696" s="32"/>
+      <c r="F696" s="32"/>
+    </row>
+    <row r="697" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A697" s="17"/>
-      <c r="B697"/>
-      <c r="C697" s="11"/>
+      <c r="B697" s="4"/>
+      <c r="C697" s="30"/>
       <c r="D697"/>
-      <c r="E697"/>
-    </row>
-    <row r="698" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E697" s="32"/>
+      <c r="F697" s="32"/>
+    </row>
+    <row r="698" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A698" s="17"/>
-      <c r="B698"/>
-      <c r="C698" s="11"/>
+      <c r="B698" s="4"/>
+      <c r="C698" s="30"/>
       <c r="D698"/>
-      <c r="E698"/>
-    </row>
-    <row r="699" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E698" s="32"/>
+      <c r="F698" s="32"/>
+    </row>
+    <row r="699" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A699" s="17"/>
-      <c r="B699"/>
-      <c r="C699" s="11"/>
+      <c r="B699" s="4"/>
+      <c r="C699" s="30"/>
       <c r="D699"/>
-      <c r="E699"/>
-    </row>
-    <row r="700" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E699" s="32"/>
+      <c r="F699" s="32"/>
+    </row>
+    <row r="700" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A700" s="17"/>
-      <c r="B700"/>
-      <c r="C700" s="11"/>
+      <c r="B700" s="4"/>
+      <c r="C700" s="30"/>
       <c r="D700"/>
-      <c r="E700"/>
-    </row>
-    <row r="701" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E700" s="32"/>
+      <c r="F700" s="32"/>
+    </row>
+    <row r="701" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A701" s="17"/>
       <c r="B701"/>
       <c r="C701" s="11"/>
       <c r="D701"/>
       <c r="E701"/>
-    </row>
-    <row r="702" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F701" s="12"/>
+    </row>
+    <row r="702" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A702" s="17"/>
       <c r="B702"/>
       <c r="C702" s="11"/>
       <c r="D702"/>
       <c r="E702"/>
-    </row>
-    <row r="703" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F702" s="12"/>
+    </row>
+    <row r="703" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A703" s="17"/>
       <c r="B703"/>
       <c r="C703" s="11"/>
       <c r="D703"/>
       <c r="E703"/>
-    </row>
-    <row r="704" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F703" s="12"/>
+    </row>
+    <row r="704" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A704" s="17"/>
       <c r="B704"/>
       <c r="C704" s="11"/>
       <c r="D704"/>
       <c r="E704"/>
-    </row>
-    <row r="705" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F704" s="12"/>
+    </row>
+    <row r="705" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A705" s="17"/>
       <c r="B705"/>
       <c r="C705" s="11"/>
       <c r="D705"/>
       <c r="E705"/>
-    </row>
-    <row r="706" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F705" s="12"/>
+    </row>
+    <row r="706" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A706" s="17"/>
       <c r="B706"/>
       <c r="C706" s="11"/>
       <c r="D706"/>
       <c r="E706"/>
-    </row>
-    <row r="707" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F706" s="12"/>
+    </row>
+    <row r="707" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A707" s="17"/>
       <c r="B707"/>
       <c r="C707" s="11"/>
       <c r="D707"/>
       <c r="E707"/>
-    </row>
-    <row r="708" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F707" s="12"/>
+    </row>
+    <row r="708" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A708" s="17"/>
       <c r="B708"/>
       <c r="C708" s="11"/>
       <c r="D708"/>
       <c r="E708"/>
-    </row>
-    <row r="709" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F708" s="12"/>
+    </row>
+    <row r="709" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A709" s="17"/>
       <c r="B709"/>
       <c r="C709" s="11"/>
       <c r="D709"/>
       <c r="E709"/>
-    </row>
-    <row r="710" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F709" s="12"/>
+    </row>
+    <row r="710" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A710" s="17"/>
       <c r="B710"/>
       <c r="C710" s="11"/>
       <c r="D710"/>
       <c r="E710"/>
-    </row>
-    <row r="711" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F710" s="12"/>
+    </row>
+    <row r="711" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A711" s="17"/>
       <c r="B711"/>
       <c r="C711" s="11"/>
       <c r="D711"/>
       <c r="E711"/>
-    </row>
-    <row r="712" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F711" s="12"/>
+    </row>
+    <row r="712" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A712" s="17"/>
       <c r="B712"/>
       <c r="C712" s="11"/>
       <c r="D712"/>
       <c r="E712"/>
-    </row>
-    <row r="713" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F712" s="12"/>
+    </row>
+    <row r="713" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A713" s="17"/>
       <c r="B713"/>
       <c r="C713" s="11"/>
       <c r="D713"/>
       <c r="E713"/>
     </row>
-    <row r="714" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A714" s="17"/>
       <c r="B714"/>
       <c r="C714" s="11"/>
       <c r="D714"/>
       <c r="E714"/>
     </row>
-    <row r="715" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A715" s="17"/>
       <c r="B715"/>
       <c r="C715" s="11"/>
       <c r="D715"/>
       <c r="E715"/>
     </row>
-    <row r="716" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="716" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A716" s="17"/>
       <c r="B716"/>
       <c r="C716" s="11"/>
       <c r="D716"/>
       <c r="E716"/>
     </row>
-    <row r="717" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="717" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A717" s="17"/>
       <c r="B717"/>
       <c r="C717" s="11"/>
       <c r="D717"/>
       <c r="E717"/>
     </row>
-    <row r="718" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="718" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A718" s="17"/>
       <c r="B718"/>
       <c r="C718" s="11"/>
       <c r="D718"/>
       <c r="E718"/>
     </row>
-    <row r="719" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="719" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A719" s="17"/>
       <c r="B719"/>
       <c r="C719" s="11"/>
       <c r="D719"/>
       <c r="E719"/>
     </row>
-    <row r="720" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A720" s="17"/>
       <c r="B720"/>
       <c r="C720" s="11"/>

</xml_diff>